<commit_message>
Rename 'dose_mg' column in all_data() to 'dose' and rename 'dose' column to 'dose_BW'
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -22,7 +22,7 @@
     <t>response</t>
   </si>
   <si>
-    <t>dose_mg</t>
+    <t>dose</t>
   </si>
   <si>
     <t>patient</t>
@@ -34,7 +34,7 @@
     <t>body_weight</t>
   </si>
   <si>
-    <t>dose</t>
+    <t>dose_BW</t>
   </si>
   <si>
     <t>7.6</t>

</xml_diff>